<commit_message>
converting prompting to per chunk instead of per review
</commit_message>
<xml_diff>
--- a/text_processing/rulebooks/TEMPLATE.xlsx
+++ b/text_processing/rulebooks/TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\individual-project-olalha\text_processing\rulebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072EE4B2-BB6A-4EF1-A0FF-C9B21D62ACD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90618344-7B6B-4F42-89AD-B1DE029B3698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34050" yWindow="3675" windowWidth="16035" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18975" yWindow="2070" windowWidth="16035" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Positive</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Room Comfort</t>
   </si>
   <si>
-    <t>Amenities</t>
-  </si>
-  <si>
     <t>Wi-Fi Quality</t>
   </si>
   <si>
@@ -101,41 +98,17 @@
     <t>Breakfast Quality</t>
   </si>
   <si>
-    <t>Room Size</t>
-  </si>
-  <si>
     <t>Parking</t>
   </si>
   <si>
-    <t>View/Scenery</t>
-  </si>
-  <si>
-    <t>Bathroom Quality</t>
-  </si>
-  <si>
-    <t>Air Conditioning/Heating</t>
-  </si>
-  <si>
-    <t>Safety &amp; Security</t>
-  </si>
-  <si>
-    <t>Booking Process</t>
-  </si>
-  <si>
-    <t>Housekeeping</t>
-  </si>
-  <si>
-    <t>Business Facilities</t>
-  </si>
-  <si>
-    <t>Family-Friendliness</t>
+    <t>Grand Plaza Hotel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +126,13 @@
     </font>
     <font>
       <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -210,7 +190,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -360,11 +340,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,6 +404,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -418,20 +437,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,144 +764,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1004"/>
+  <dimension ref="A1:G1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="21" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="15" customWidth="1"/>
     <col min="3" max="5" width="12.7109375" style="9" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="12" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="17"/>
-    </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="str">
-        <f>IF(SUM(B4:B1048576)=1,"VALID","INVALID")</f>
+      <c r="B3" s="8" t="str">
+        <f>IF(SUM(B5:B1048576)=1,"VALID","INVALID")</f>
         <v>VALID</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="8" t="str">
-        <f>IF(COUNTIF(G4:G1048576, "INVALID")&gt;0, "INVALID", "VALID")</f>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="8" t="str">
+        <f>IF(COUNTIF(G5:G1048576, "INVALID")&gt;0, "INVALID", "VALID")</f>
         <v>VALID</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="5" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B5" s="16">
         <v>0.13</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C5" s="9">
         <v>0.8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D5" s="9">
         <v>0.1</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E5" s="9">
         <v>0.1</v>
       </c>
-      <c r="F4" s="12">
-        <f>IF(B4&lt;&gt;"", SUM(ABS(C4), ABS(D4), ABS(E4)), "")</f>
+      <c r="F5" s="12">
+        <f>IF(B5&lt;&gt;"", SUM(ABS(C5), ABS(D5), ABS(E5)), "")</f>
         <v>1</v>
       </c>
-      <c r="G4" s="10" t="str">
-        <f t="shared" ref="G4:G67" si="0">IF(F4&lt;&gt;"", IF(AND(F4=1, C4&lt;&gt;"", D4&lt;&gt;"", E4&lt;&gt;"", B4&gt;=0, B4&lt;=1), "VALID", "INVALID"), "")</f>
+      <c r="G5" s="10" t="str">
+        <f t="shared" ref="G5:G68" si="0">IF(F5&lt;&gt;"", IF(AND(F5=1, C5&lt;&gt;"", D5&lt;&gt;"", E5&lt;&gt;"", B5&gt;=0, B5&lt;=1), "VALID", "INVALID"), "")</f>
         <v>VALID</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B6" s="17">
         <v>0.25</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C6" s="9">
         <v>0.5</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D6" s="9">
         <v>0.2</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="9">
         <v>0.3</v>
       </c>
-      <c r="F5" s="12">
-        <f t="shared" ref="F5:F68" si="1">IF(B5&lt;&gt;"", SUM(ABS(C5), ABS(D5), ABS(E5)), "")</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="11" t="str">
-        <f t="shared" si="0"/>
-        <v>VALID</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="23">
-        <v>0.02</v>
-      </c>
-      <c r="C6" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
       <c r="F6" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F6:F69" si="1">IF(B6&lt;&gt;"", SUM(ABS(C6), ABS(D6), ABS(E6)), "")</f>
         <v>1</v>
       </c>
       <c r="G6" s="11" t="str">
@@ -900,20 +896,20 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="23">
-        <v>0.12</v>
+      <c r="A7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0.02</v>
       </c>
       <c r="C7" s="9">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="9">
-        <v>0.15</v>
+        <v>0.8</v>
       </c>
       <c r="E7" s="9">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="1"/>
@@ -925,20 +921,20 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="23">
-        <v>0.01</v>
+      <c r="A8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0.12</v>
       </c>
       <c r="C8" s="9">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D8" s="9">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E8" s="9">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" si="1"/>
@@ -950,20 +946,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="23">
-        <v>0.14000000000000001</v>
+      <c r="A9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0.05</v>
       </c>
       <c r="C9" s="9">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D9" s="9">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E9" s="9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="1"/>
@@ -975,20 +971,20 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="23">
-        <v>0.12</v>
+      <c r="A10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="17">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C10" s="9">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D10" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="E10" s="9">
         <v>0.4</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.1</v>
       </c>
       <c r="F10" s="12">
         <f t="shared" si="1"/>
@@ -1000,20 +996,20 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="23">
+      <c r="A11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="17">
         <v>0.12</v>
       </c>
       <c r="C11" s="9">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E11" s="9">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="F11" s="12">
         <f t="shared" si="1"/>
@@ -1025,20 +1021,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="23">
-        <v>0.02</v>
+      <c r="A12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="17">
+        <v>0.08</v>
       </c>
       <c r="C12" s="9">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D12" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="9">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F12" s="12">
         <f t="shared" si="1"/>
@@ -1050,20 +1046,20 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="23">
-        <v>7.0000000000000007E-2</v>
+      <c r="A13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="17">
+        <v>0.02</v>
       </c>
       <c r="C13" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="9">
         <v>0</v>
       </c>
       <c r="E13" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="1"/>
@@ -1075,17 +1071,17 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="21">
+      <c r="A14" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="17">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
         <v>0</v>
-      </c>
-      <c r="C14" s="9">
-        <v>0</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1</v>
       </c>
       <c r="E14" s="9">
         <v>0</v>
@@ -1100,231 +1096,106 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="21">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
-        <v>0</v>
-      </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="12">
+      <c r="A15" s="14"/>
+      <c r="F15" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G15" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="21">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12">
+      <c r="A16" s="14"/>
+      <c r="F16" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G16" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="21">
-        <v>0</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9">
-        <v>0</v>
-      </c>
-      <c r="F17" s="12">
+      <c r="A17" s="14"/>
+      <c r="F17" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G17" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="21">
-        <v>0</v>
-      </c>
-      <c r="C18" s="9">
-        <v>0</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12">
+      <c r="A18" s="14"/>
+      <c r="F18" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G18" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="21">
-        <v>0</v>
-      </c>
-      <c r="C19" s="9">
-        <v>0</v>
-      </c>
-      <c r="D19" s="9">
-        <v>1</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
+      <c r="A19" s="14"/>
+      <c r="F19" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G19" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="21">
-        <v>0</v>
-      </c>
-      <c r="C20" s="9">
-        <v>0</v>
-      </c>
-      <c r="D20" s="9">
-        <v>1</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
+      <c r="A20" s="14"/>
+      <c r="F20" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G20" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="21">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0</v>
-      </c>
-      <c r="F21" s="12">
+      <c r="A21" s="14"/>
+      <c r="F21" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G21" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="21">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0</v>
-      </c>
-      <c r="D22" s="9">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0</v>
-      </c>
-      <c r="F22" s="12">
+      <c r="A22" s="14"/>
+      <c r="F22" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G22" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="21">
-        <v>0</v>
-      </c>
-      <c r="C23" s="9">
-        <v>0</v>
-      </c>
-      <c r="D23" s="9">
-        <v>1</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0</v>
-      </c>
-      <c r="F23" s="12">
+      <c r="A23" s="14"/>
+      <c r="F23" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="G23" s="11" t="str">
         <f t="shared" si="0"/>
-        <v>VALID</v>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
       <c r="F24" s="12" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1770,23 +1641,23 @@
         <v/>
       </c>
       <c r="G68" s="11" t="str">
-        <f t="shared" ref="G68:G131" si="2">IF(F68&lt;&gt;"", IF(AND(F68=1, C68&lt;&gt;"", D68&lt;&gt;"", E68&lt;&gt;"", B68&gt;=0, B68&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F69" s="12" t="str">
-        <f t="shared" ref="F69:F132" si="3">IF(B69&lt;&gt;"", SUM(ABS(C69), ABS(D69), ABS(E69)), "")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G69" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G69:G132" si="2">IF(F69&lt;&gt;"", IF(AND(F69=1, C69&lt;&gt;"", D69&lt;&gt;"", E69&lt;&gt;"", B69&gt;=0, B69&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F70" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F70:F133" si="3">IF(B70&lt;&gt;"", SUM(ABS(C70), ABS(D70), ABS(E70)), "")</f>
         <v/>
       </c>
       <c r="G70" s="11" t="str">
@@ -2410,23 +2281,23 @@
         <v/>
       </c>
       <c r="G132" s="11" t="str">
-        <f t="shared" ref="G132:G195" si="4">IF(F132&lt;&gt;"", IF(AND(F132=1, C132&lt;&gt;"", D132&lt;&gt;"", E132&lt;&gt;"", B132&gt;=0, B132&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F133" s="12" t="str">
-        <f t="shared" ref="F133:F196" si="5">IF(B133&lt;&gt;"", SUM(ABS(C133), ABS(D133), ABS(E133)), "")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="G133" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G133:G196" si="4">IF(F133&lt;&gt;"", IF(AND(F133=1, C133&lt;&gt;"", D133&lt;&gt;"", E133&lt;&gt;"", B133&gt;=0, B133&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="134" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F134" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F134:F197" si="5">IF(B134&lt;&gt;"", SUM(ABS(C134), ABS(D134), ABS(E134)), "")</f>
         <v/>
       </c>
       <c r="G134" s="11" t="str">
@@ -3050,23 +2921,23 @@
         <v/>
       </c>
       <c r="G196" s="11" t="str">
-        <f t="shared" ref="G196:G259" si="6">IF(F196&lt;&gt;"", IF(AND(F196=1, C196&lt;&gt;"", D196&lt;&gt;"", E196&lt;&gt;"", B196&gt;=0, B196&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="197" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F197" s="12" t="str">
-        <f t="shared" ref="F197:F260" si="7">IF(B197&lt;&gt;"", SUM(ABS(C197), ABS(D197), ABS(E197)), "")</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="G197" s="11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="G197:G260" si="6">IF(F197&lt;&gt;"", IF(AND(F197=1, C197&lt;&gt;"", D197&lt;&gt;"", E197&lt;&gt;"", B197&gt;=0, B197&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="198" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F198" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="F198:F261" si="7">IF(B198&lt;&gt;"", SUM(ABS(C198), ABS(D198), ABS(E198)), "")</f>
         <v/>
       </c>
       <c r="G198" s="11" t="str">
@@ -3690,23 +3561,23 @@
         <v/>
       </c>
       <c r="G260" s="11" t="str">
-        <f t="shared" ref="G260:G323" si="8">IF(F260&lt;&gt;"", IF(AND(F260=1, C260&lt;&gt;"", D260&lt;&gt;"", E260&lt;&gt;"", B260&gt;=0, B260&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="261" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F261" s="12" t="str">
-        <f t="shared" ref="F261:F324" si="9">IF(B261&lt;&gt;"", SUM(ABS(C261), ABS(D261), ABS(E261)), "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="G261" s="11" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="G261:G324" si="8">IF(F261&lt;&gt;"", IF(AND(F261=1, C261&lt;&gt;"", D261&lt;&gt;"", E261&lt;&gt;"", B261&gt;=0, B261&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="262" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F262" s="12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="F262:F325" si="9">IF(B262&lt;&gt;"", SUM(ABS(C262), ABS(D262), ABS(E262)), "")</f>
         <v/>
       </c>
       <c r="G262" s="11" t="str">
@@ -4330,23 +4201,23 @@
         <v/>
       </c>
       <c r="G324" s="11" t="str">
-        <f t="shared" ref="G324:G387" si="10">IF(F324&lt;&gt;"", IF(AND(F324=1, C324&lt;&gt;"", D324&lt;&gt;"", E324&lt;&gt;"", B324&gt;=0, B324&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
     <row r="325" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F325" s="12" t="str">
-        <f t="shared" ref="F325:F388" si="11">IF(B325&lt;&gt;"", SUM(ABS(C325), ABS(D325), ABS(E325)), "")</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G325" s="11" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G325:G388" si="10">IF(F325&lt;&gt;"", IF(AND(F325=1, C325&lt;&gt;"", D325&lt;&gt;"", E325&lt;&gt;"", B325&gt;=0, B325&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="326" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F326" s="12" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="F326:F389" si="11">IF(B326&lt;&gt;"", SUM(ABS(C326), ABS(D326), ABS(E326)), "")</f>
         <v/>
       </c>
       <c r="G326" s="11" t="str">
@@ -4970,23 +4841,23 @@
         <v/>
       </c>
       <c r="G388" s="11" t="str">
-        <f t="shared" ref="G388:G451" si="12">IF(F388&lt;&gt;"", IF(AND(F388=1, C388&lt;&gt;"", D388&lt;&gt;"", E388&lt;&gt;"", B388&gt;=0, B388&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
     </row>
     <row r="389" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F389" s="12" t="str">
-        <f t="shared" ref="F389:F452" si="13">IF(B389&lt;&gt;"", SUM(ABS(C389), ABS(D389), ABS(E389)), "")</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G389" s="11" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="G389:G452" si="12">IF(F389&lt;&gt;"", IF(AND(F389=1, C389&lt;&gt;"", D389&lt;&gt;"", E389&lt;&gt;"", B389&gt;=0, B389&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="390" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F390" s="12" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="F390:F453" si="13">IF(B390&lt;&gt;"", SUM(ABS(C390), ABS(D390), ABS(E390)), "")</f>
         <v/>
       </c>
       <c r="G390" s="11" t="str">
@@ -5610,23 +5481,23 @@
         <v/>
       </c>
       <c r="G452" s="11" t="str">
-        <f t="shared" ref="G452:G515" si="14">IF(F452&lt;&gt;"", IF(AND(F452=1, C452&lt;&gt;"", D452&lt;&gt;"", E452&lt;&gt;"", B452&gt;=0, B452&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
     </row>
     <row r="453" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F453" s="12" t="str">
-        <f t="shared" ref="F453:F516" si="15">IF(B453&lt;&gt;"", SUM(ABS(C453), ABS(D453), ABS(E453)), "")</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G453" s="11" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="G453:G516" si="14">IF(F453&lt;&gt;"", IF(AND(F453=1, C453&lt;&gt;"", D453&lt;&gt;"", E453&lt;&gt;"", B453&gt;=0, B453&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="454" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F454" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="F454:F517" si="15">IF(B454&lt;&gt;"", SUM(ABS(C454), ABS(D454), ABS(E454)), "")</f>
         <v/>
       </c>
       <c r="G454" s="11" t="str">
@@ -6250,23 +6121,23 @@
         <v/>
       </c>
       <c r="G516" s="11" t="str">
-        <f t="shared" ref="G516:G579" si="16">IF(F516&lt;&gt;"", IF(AND(F516=1, C516&lt;&gt;"", D516&lt;&gt;"", E516&lt;&gt;"", B516&gt;=0, B516&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
     <row r="517" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F517" s="12" t="str">
-        <f t="shared" ref="F517:F580" si="17">IF(B517&lt;&gt;"", SUM(ABS(C517), ABS(D517), ABS(E517)), "")</f>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G517" s="11" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="G517:G580" si="16">IF(F517&lt;&gt;"", IF(AND(F517=1, C517&lt;&gt;"", D517&lt;&gt;"", E517&lt;&gt;"", B517&gt;=0, B517&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="518" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F518" s="12" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="F518:F581" si="17">IF(B518&lt;&gt;"", SUM(ABS(C518), ABS(D518), ABS(E518)), "")</f>
         <v/>
       </c>
       <c r="G518" s="11" t="str">
@@ -6890,23 +6761,23 @@
         <v/>
       </c>
       <c r="G580" s="11" t="str">
-        <f t="shared" ref="G580:G643" si="18">IF(F580&lt;&gt;"", IF(AND(F580=1, C580&lt;&gt;"", D580&lt;&gt;"", E580&lt;&gt;"", B580&gt;=0, B580&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
     <row r="581" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F581" s="12" t="str">
-        <f t="shared" ref="F581:F644" si="19">IF(B581&lt;&gt;"", SUM(ABS(C581), ABS(D581), ABS(E581)), "")</f>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="G581" s="11" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="G581:G644" si="18">IF(F581&lt;&gt;"", IF(AND(F581=1, C581&lt;&gt;"", D581&lt;&gt;"", E581&lt;&gt;"", B581&gt;=0, B581&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="582" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F582" s="12" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="F582:F645" si="19">IF(B582&lt;&gt;"", SUM(ABS(C582), ABS(D582), ABS(E582)), "")</f>
         <v/>
       </c>
       <c r="G582" s="11" t="str">
@@ -7530,23 +7401,23 @@
         <v/>
       </c>
       <c r="G644" s="11" t="str">
-        <f t="shared" ref="G644:G707" si="20">IF(F644&lt;&gt;"", IF(AND(F644=1, C644&lt;&gt;"", D644&lt;&gt;"", E644&lt;&gt;"", B644&gt;=0, B644&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
     <row r="645" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F645" s="12" t="str">
-        <f t="shared" ref="F645:F708" si="21">IF(B645&lt;&gt;"", SUM(ABS(C645), ABS(D645), ABS(E645)), "")</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="G645" s="11" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="G645:G708" si="20">IF(F645&lt;&gt;"", IF(AND(F645=1, C645&lt;&gt;"", D645&lt;&gt;"", E645&lt;&gt;"", B645&gt;=0, B645&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="646" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F646" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="F646:F709" si="21">IF(B646&lt;&gt;"", SUM(ABS(C646), ABS(D646), ABS(E646)), "")</f>
         <v/>
       </c>
       <c r="G646" s="11" t="str">
@@ -8170,23 +8041,23 @@
         <v/>
       </c>
       <c r="G708" s="11" t="str">
-        <f t="shared" ref="G708:G771" si="22">IF(F708&lt;&gt;"", IF(AND(F708=1, C708&lt;&gt;"", D708&lt;&gt;"", E708&lt;&gt;"", B708&gt;=0, B708&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="709" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F709" s="12" t="str">
-        <f t="shared" ref="F709:F772" si="23">IF(B709&lt;&gt;"", SUM(ABS(C709), ABS(D709), ABS(E709)), "")</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="G709" s="11" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="G709:G772" si="22">IF(F709&lt;&gt;"", IF(AND(F709=1, C709&lt;&gt;"", D709&lt;&gt;"", E709&lt;&gt;"", B709&gt;=0, B709&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="710" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F710" s="12" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="F710:F773" si="23">IF(B710&lt;&gt;"", SUM(ABS(C710), ABS(D710), ABS(E710)), "")</f>
         <v/>
       </c>
       <c r="G710" s="11" t="str">
@@ -8810,23 +8681,23 @@
         <v/>
       </c>
       <c r="G772" s="11" t="str">
-        <f t="shared" ref="G772:G835" si="24">IF(F772&lt;&gt;"", IF(AND(F772=1, C772&lt;&gt;"", D772&lt;&gt;"", E772&lt;&gt;"", B772&gt;=0, B772&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="773" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F773" s="12" t="str">
-        <f t="shared" ref="F773:F836" si="25">IF(B773&lt;&gt;"", SUM(ABS(C773), ABS(D773), ABS(E773)), "")</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="G773" s="11" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="G773:G836" si="24">IF(F773&lt;&gt;"", IF(AND(F773=1, C773&lt;&gt;"", D773&lt;&gt;"", E773&lt;&gt;"", B773&gt;=0, B773&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="774" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F774" s="12" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="F774:F837" si="25">IF(B774&lt;&gt;"", SUM(ABS(C774), ABS(D774), ABS(E774)), "")</f>
         <v/>
       </c>
       <c r="G774" s="11" t="str">
@@ -9450,23 +9321,23 @@
         <v/>
       </c>
       <c r="G836" s="11" t="str">
-        <f t="shared" ref="G836:G899" si="26">IF(F836&lt;&gt;"", IF(AND(F836=1, C836&lt;&gt;"", D836&lt;&gt;"", E836&lt;&gt;"", B836&gt;=0, B836&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
     <row r="837" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F837" s="12" t="str">
-        <f t="shared" ref="F837:F900" si="27">IF(B837&lt;&gt;"", SUM(ABS(C837), ABS(D837), ABS(E837)), "")</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="G837" s="11" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" ref="G837:G900" si="26">IF(F837&lt;&gt;"", IF(AND(F837=1, C837&lt;&gt;"", D837&lt;&gt;"", E837&lt;&gt;"", B837&gt;=0, B837&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="838" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F838" s="12" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" ref="F838:F901" si="27">IF(B838&lt;&gt;"", SUM(ABS(C838), ABS(D838), ABS(E838)), "")</f>
         <v/>
       </c>
       <c r="G838" s="11" t="str">
@@ -10090,23 +9961,23 @@
         <v/>
       </c>
       <c r="G900" s="11" t="str">
-        <f t="shared" ref="G900:G963" si="28">IF(F900&lt;&gt;"", IF(AND(F900=1, C900&lt;&gt;"", D900&lt;&gt;"", E900&lt;&gt;"", B900&gt;=0, B900&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
     <row r="901" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F901" s="12" t="str">
-        <f t="shared" ref="F901:F964" si="29">IF(B901&lt;&gt;"", SUM(ABS(C901), ABS(D901), ABS(E901)), "")</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="G901" s="11" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" ref="G901:G964" si="28">IF(F901&lt;&gt;"", IF(AND(F901=1, C901&lt;&gt;"", D901&lt;&gt;"", E901&lt;&gt;"", B901&gt;=0, B901&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="902" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F902" s="12" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" ref="F902:F965" si="29">IF(B902&lt;&gt;"", SUM(ABS(C902), ABS(D902), ABS(E902)), "")</f>
         <v/>
       </c>
       <c r="G902" s="11" t="str">
@@ -10730,23 +10601,23 @@
         <v/>
       </c>
       <c r="G964" s="11" t="str">
-        <f t="shared" ref="G964:G1004" si="30">IF(F964&lt;&gt;"", IF(AND(F964=1, C964&lt;&gt;"", D964&lt;&gt;"", E964&lt;&gt;"", B964&gt;=0, B964&lt;=1), "VALID", "INVALID"), "")</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
     </row>
     <row r="965" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F965" s="12" t="str">
-        <f t="shared" ref="F965:F1004" si="31">IF(B965&lt;&gt;"", SUM(ABS(C965), ABS(D965), ABS(E965)), "")</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="G965" s="11" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" ref="G965:G1005" si="30">IF(F965&lt;&gt;"", IF(AND(F965=1, C965&lt;&gt;"", D965&lt;&gt;"", E965&lt;&gt;"", B965&gt;=0, B965&lt;=1), "VALID", "INVALID"), "")</f>
         <v/>
       </c>
     </row>
     <row r="966" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F966" s="12" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" ref="F966:F1005" si="31">IF(B966&lt;&gt;"", SUM(ABS(C966), ABS(D966), ABS(E966)), "")</f>
         <v/>
       </c>
       <c r="G966" s="11" t="str">
@@ -11134,13 +11005,24 @@
         <v/>
       </c>
     </row>
+    <row r="1005" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F1005" s="12" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="G1005" s="11" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C2:F2"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2 G2">
+  <conditionalFormatting sqref="B3 G3">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"VALID"</formula>
     </cfRule>
@@ -11148,7 +11030,7 @@
       <formula>"INVALID"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G1048576">
+  <conditionalFormatting sqref="G5:G1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"VALID"</formula>
     </cfRule>

</xml_diff>